<commit_message>
familiarity reviews coming to an end
</commit_message>
<xml_diff>
--- a/familiarity review/SystemLevelTests/AmazonTest.xlsx
+++ b/familiarity review/SystemLevelTests/AmazonTest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CIT360-OOP\isaac-ireland.github.io\familiarity review\SystemLevelTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00875AA9-4DBF-44ED-887C-F78847EAC16C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D938B6-F9E4-4283-B64A-EDC46DA8D800}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{130DBBC9-4ADF-47FE-989D-9D6F56E328E9}"/>
+    <workbookView xWindow="-15870" yWindow="-6615" windowWidth="15990" windowHeight="24840" xr2:uid="{130DBBC9-4ADF-47FE-989D-9D6F56E328E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -237,9 +237,6 @@
     <t>email</t>
   </si>
   <si>
-    <t>email, not readily accessable,</t>
-  </si>
-  <si>
     <t>Submit Feeback</t>
   </si>
   <si>
@@ -276,7 +273,10 @@
     <t>Veriety of milks available</t>
   </si>
   <si>
-    <t>Not sure if specific item is sold, Funiture Stencils did exist, did not recommend them</t>
+    <t>Not sure if specific item is sold, Furniture Stencils did exist, did not recommend them</t>
+  </si>
+  <si>
+    <t>email, not readily accessible,</t>
   </si>
 </sst>
 </file>
@@ -364,10 +364,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -376,7 +373,10 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="1" applyAlignment="1">
@@ -700,7 +700,7 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H35"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -729,72 +729,72 @@
       <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="7" t="s">
+      <c r="D4" s="9"/>
+      <c r="E4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="7"/>
+      <c r="F4" s="10"/>
       <c r="G4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="7" t="s">
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="7"/>
+      <c r="F5" s="10"/>
       <c r="G5" s="5">
         <v>0.625</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="6" t="s">
+      <c r="B6" s="10"/>
+      <c r="C6" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -803,10 +803,10 @@
       <c r="B7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="9"/>
+      <c r="D7" s="8"/>
       <c r="E7" s="3" t="s">
         <v>16</v>
       </c>
@@ -821,10 +821,10 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="8"/>
+      <c r="B8" s="7"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -833,10 +833,10 @@
       <c r="B9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="6"/>
+      <c r="D9" s="9"/>
       <c r="E9" t="s">
         <v>63</v>
       </c>
@@ -848,10 +848,10 @@
       <c r="B10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="6"/>
+      <c r="D10" s="9"/>
       <c r="E10" t="s">
         <v>63</v>
       </c>
@@ -863,10 +863,10 @@
       <c r="B11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="6"/>
+      <c r="D11" s="9"/>
       <c r="E11" t="s">
         <v>63</v>
       </c>
@@ -878,10 +878,10 @@
       <c r="B12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="D12" s="6"/>
+      <c r="D12" s="9"/>
       <c r="E12" t="s">
         <v>63</v>
       </c>
@@ -893,10 +893,10 @@
       <c r="B13" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="6"/>
+      <c r="D13" s="9"/>
       <c r="E13" t="s">
         <v>63</v>
       </c>
@@ -908,10 +908,10 @@
       <c r="B14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="D14" s="6"/>
+      <c r="D14" s="9"/>
       <c r="E14" t="s">
         <v>63</v>
       </c>
@@ -923,10 +923,10 @@
       <c r="B15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="6"/>
+      <c r="D15" s="9"/>
       <c r="E15" t="s">
         <v>63</v>
       </c>
@@ -938,15 +938,15 @@
       <c r="B16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D16" s="6"/>
+      <c r="D16" s="9"/>
       <c r="E16" t="s">
         <v>63</v>
       </c>
       <c r="H16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -956,22 +956,22 @@
       <c r="B17" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="6"/>
+      <c r="D17" s="9"/>
       <c r="E17" t="s">
         <v>63</v>
       </c>
       <c r="H17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="10"/>
+      <c r="B18" s="6"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
@@ -987,7 +987,7 @@
         <v>63</v>
       </c>
       <c r="H19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1004,7 +1004,7 @@
         <v>63</v>
       </c>
       <c r="H20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1021,7 +1021,7 @@
         <v>63</v>
       </c>
       <c r="H21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1038,7 +1038,7 @@
         <v>63</v>
       </c>
       <c r="H22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1055,7 +1055,7 @@
         <v>63</v>
       </c>
       <c r="H23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1072,7 +1072,7 @@
         <v>63</v>
       </c>
       <c r="H24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1109,14 +1109,14 @@
         <v>63</v>
       </c>
       <c r="H26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="10"/>
+      <c r="B27" s="6"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
@@ -1149,7 +1149,7 @@
         <v>63</v>
       </c>
       <c r="H29" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -1187,17 +1187,17 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="B32" s="10"/>
+      <c r="A32" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" s="6"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>22</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E33" t="s">
         <v>63</v>
@@ -1208,7 +1208,7 @@
         <v>23</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E34" t="s">
         <v>63</v>
@@ -1219,7 +1219,7 @@
         <v>24</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E35" t="s">
         <v>63</v>
@@ -1227,6 +1227,16 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:H6"/>
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="C7:D7"/>
@@ -1241,16 +1251,6 @@
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:H6"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="C2:H2"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="C4:D4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Proffessional Behavior basis 1
</commit_message>
<xml_diff>
--- a/familiarity review/SystemLevelTests/AmazonTest.xlsx
+++ b/familiarity review/SystemLevelTests/AmazonTest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CIT360-OOP\isaac-ireland.github.io\familiarity review\SystemLevelTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D938B6-F9E4-4283-B64A-EDC46DA8D800}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0E12EBE-CA26-49DD-8417-4A63F0BFFA23}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15870" yWindow="-6615" windowWidth="15990" windowHeight="24840" xr2:uid="{130DBBC9-4ADF-47FE-989D-9D6F56E328E9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{130DBBC9-4ADF-47FE-989D-9D6F56E328E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="93">
   <si>
     <t>amazon store</t>
   </si>
@@ -78,9 +78,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Expected Results</t>
-  </si>
-  <si>
     <t>Pass</t>
   </si>
   <si>
@@ -159,54 +156,9 @@
     <t>Text/chat Amazon</t>
   </si>
   <si>
-    <t>Easy find, simple</t>
-  </si>
-  <si>
-    <t>As easy as login</t>
-  </si>
-  <si>
-    <t>item found in cart</t>
-  </si>
-  <si>
     <t>remove from history</t>
   </si>
   <si>
-    <t>don’t need related items</t>
-  </si>
-  <si>
-    <t>item not in cart</t>
-  </si>
-  <si>
-    <t>email confirming order</t>
-  </si>
-  <si>
-    <t>Billed and shipped</t>
-  </si>
-  <si>
-    <t>not directly in cart</t>
-  </si>
-  <si>
-    <t>back in cart</t>
-  </si>
-  <si>
-    <t>Horror</t>
-  </si>
-  <si>
-    <t>Harry Potter</t>
-  </si>
-  <si>
-    <t>Car Fuse</t>
-  </si>
-  <si>
-    <t>NEMA 14</t>
-  </si>
-  <si>
-    <t>Milk</t>
-  </si>
-  <si>
-    <t>Pane of heat risistance glass for 3D printer</t>
-  </si>
-  <si>
     <t>Be able to call Amazon</t>
   </si>
   <si>
@@ -216,24 +168,12 @@
     <t>Incorrect Item delivered</t>
   </si>
   <si>
-    <t>Follow the Music</t>
-  </si>
-  <si>
-    <t>Timely No T-132 Furniture Stencil</t>
-  </si>
-  <si>
     <t>*</t>
   </si>
   <si>
     <t xml:space="preserve">Adds were good, but search engine did not understand </t>
   </si>
   <si>
-    <t>only 6 Clicks, Good Job</t>
-  </si>
-  <si>
-    <t>Not Very Visable, UX seemingly intentionaly off</t>
-  </si>
-  <si>
     <t>email</t>
   </si>
   <si>
@@ -255,9 +195,6 @@
     <t>Reasonable time till email sent</t>
   </si>
   <si>
-    <t>Books on 1st Page</t>
-  </si>
-  <si>
     <t>Good</t>
   </si>
   <si>
@@ -273,10 +210,106 @@
     <t>Veriety of milks available</t>
   </si>
   <si>
-    <t>Not sure if specific item is sold, Furniture Stencils did exist, did not recommend them</t>
-  </si>
-  <si>
-    <t>email, not readily accessible,</t>
+    <t>As easy as login/ found under account&amp; Lists: acconut</t>
+  </si>
+  <si>
+    <t>Expected Results/where accessed in test</t>
+  </si>
+  <si>
+    <t>Easy find, simple/ auto Log-in, no password asked</t>
+  </si>
+  <si>
+    <t>item found in cart/ use recommended item on landing page: use add to cart, not "Buy now" option</t>
+  </si>
+  <si>
+    <t>item not in cart/ remove while in cart window, select "delete" under item</t>
+  </si>
+  <si>
+    <t>Item most recently added to cart and looked up not there</t>
+  </si>
+  <si>
+    <t>don’t need related items/ go to browsing history on banner, select history and select "remove from view"</t>
+  </si>
+  <si>
+    <t>not directly in cart/ go to cart while item is in it, and select "Save for later" next to "delete" on itme</t>
+  </si>
+  <si>
+    <t>back in cart/ while in "cart" page, find the item you want and select "move to cart"</t>
+  </si>
+  <si>
+    <t>Billed and shipped/ with item in cart, select the yellow "proceed to checkout", use correct address, payment method, and shipping and than select "place your order"</t>
+  </si>
+  <si>
+    <t>email confirming order/ check email after 5 minutes and see if confirmation email is there</t>
+  </si>
+  <si>
+    <t>Harry Potter/ in all</t>
+  </si>
+  <si>
+    <t>Books on 1st Page, some other items that are harry potter themed</t>
+  </si>
+  <si>
+    <t>term searched for/ category searched on</t>
+  </si>
+  <si>
+    <t>Horror/ in Kindle Store</t>
+  </si>
+  <si>
+    <t>Follow the Music/ in Kindle store</t>
+  </si>
+  <si>
+    <t>Car Fuse/ all</t>
+  </si>
+  <si>
+    <t>NEMA 14/All</t>
+  </si>
+  <si>
+    <t>Milk/all</t>
+  </si>
+  <si>
+    <t>Pane of heat risistance glass for 3D printer/all</t>
+  </si>
+  <si>
+    <t>Timely No T-132 Furniture Stencil/ all</t>
+  </si>
+  <si>
+    <t>Overly Specific 3</t>
+  </si>
+  <si>
+    <t>Furniture Stencil/ all</t>
+  </si>
+  <si>
+    <t>Found what I was looking for, a stencil for making furniture in blueprints</t>
+  </si>
+  <si>
+    <t>Furniture Stencils did exist, but did not recommend any of them, even if they did not have the timely No T-123</t>
+  </si>
+  <si>
+    <t>only 6 Clicks, Good Job/ found by selecting Orders: problem with Order: Different from what I orderd: Contact Seller</t>
+  </si>
+  <si>
+    <t>Not Very Visable, UX seemingly intentionaly off/ Looked under Help; need more help; contact us; devices; select device; select some categories; chat</t>
+  </si>
+  <si>
+    <t>Not Very Visable, UX seemingly intentionaly off/Looked under Help; need more help; contact us; devices; select device; select some categories; chat</t>
+  </si>
+  <si>
+    <t>email, not readily accessible could not find in my searches</t>
+  </si>
+  <si>
+    <t>selected "my account" sub item "my orders": scroll to item in question and select "leave seller feedback": sign in if needed and leave review  including stars and comments</t>
+  </si>
+  <si>
+    <t>feedback on puzzle ordered before by "American gift source"</t>
+  </si>
+  <si>
+    <t>looked at Buffalo Games</t>
+  </si>
+  <si>
+    <t>when on an item selected the name after "by" this is the retailer selling the items</t>
+  </si>
+  <si>
+    <t>for security reasons Amazon will not let you email a seller directly send a message by: selecting the "seller feedback" of the item you have questions about in your order's; then select the yellow button labled "ask a question" there are a limited reasons Amazon has for writing a message, but a rudimentary option to contact them is there.</t>
   </si>
 </sst>
 </file>
@@ -299,7 +332,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -341,6 +374,12 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -355,7 +394,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -364,6 +403,15 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -373,15 +421,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -697,104 +737,103 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDEDABBC-21CF-49A8-B0E2-CA1FB9575ACE}">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18.42578125" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" customWidth="1"/>
+    <col min="3" max="4" width="33.42578125" customWidth="1"/>
     <col min="7" max="7" width="10.140625" customWidth="1"/>
     <col min="8" max="8" width="27.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="10" t="s">
+      <c r="D4" s="7"/>
+      <c r="E4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="10"/>
+      <c r="F4" s="8"/>
       <c r="G4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="10" t="s">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="10"/>
+      <c r="F5" s="8"/>
       <c r="G5" s="5">
         <v>0.625</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="9" t="s">
+      <c r="B6" s="8"/>
+      <c r="C6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -803,42 +842,42 @@
       <c r="B7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="11"/>
+      <c r="E7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="G7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="H7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="3" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="7"/>
+      <c r="B8" s="10"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="9"/>
+        <v>19</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="7"/>
       <c r="E9" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -846,14 +885,14 @@
         <v>2</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" s="9"/>
+        <v>20</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="7"/>
       <c r="E10" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -861,14 +900,14 @@
         <v>3</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" s="9"/>
+        <v>21</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" s="7"/>
       <c r="E11" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -876,14 +915,14 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="D12" s="9"/>
+        <v>22</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="7"/>
       <c r="E12" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -891,14 +930,17 @@
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D13" s="9"/>
+        <v>41</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" s="7"/>
       <c r="E13" t="s">
-        <v>63</v>
+        <v>45</v>
+      </c>
+      <c r="H13" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -906,14 +948,14 @@
         <v>6</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D14" s="9"/>
+        <v>23</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="7"/>
       <c r="E14" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -921,14 +963,14 @@
         <v>7</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" s="9"/>
+        <v>24</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" s="7"/>
       <c r="E15" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -936,17 +978,17 @@
         <v>8</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D16" s="9"/>
+        <v>25</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="7"/>
       <c r="E16" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="H16" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -954,40 +996,44 @@
         <v>9</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" s="7"/>
+      <c r="E17" t="s">
+        <v>45</v>
+      </c>
+      <c r="H17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="D17" s="9"/>
-      <c r="E17" t="s">
-        <v>63</v>
-      </c>
-      <c r="H17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="6"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" s="12"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>10</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C19" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="E19" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="H19" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -995,16 +1041,16 @@
         <v>11</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C20" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="E20" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="H20" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1012,16 +1058,16 @@
         <v>12</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C21" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="E21" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="H21" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1029,16 +1075,16 @@
         <v>13</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C22" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="E22" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="H22" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1046,16 +1092,16 @@
         <v>14</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C23" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="E23" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="H23" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1063,16 +1109,16 @@
         <v>15</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C24" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="E24" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="H24" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1080,16 +1126,16 @@
         <v>16</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C25" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="F25" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="H25" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1097,59 +1143,56 @@
         <v>17</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C26" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="F26" t="s">
-        <v>63</v>
-      </c>
-      <c r="G26" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="H26" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>18</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B27" s="6"/>
+      <c r="C27" t="s">
+        <v>81</v>
+      </c>
+      <c r="E27" t="s">
+        <v>45</v>
+      </c>
+      <c r="H27" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
-        <v>18</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C28" t="s">
-        <v>60</v>
-      </c>
-      <c r="E28" t="s">
-        <v>63</v>
-      </c>
-      <c r="H28" t="s">
-        <v>65</v>
-      </c>
+      <c r="A28" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="9"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>19</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C29" t="s">
-        <v>67</v>
-      </c>
-      <c r="F29" t="s">
-        <v>63</v>
+        <v>44</v>
+      </c>
+      <c r="E29" t="s">
+        <v>45</v>
       </c>
       <c r="H29" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -1157,16 +1200,16 @@
         <v>20</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C30" t="s">
-        <v>58</v>
-      </c>
-      <c r="E30" t="s">
-        <v>63</v>
+        <v>47</v>
+      </c>
+      <c r="F30" t="s">
+        <v>45</v>
       </c>
       <c r="H30" t="s">
-        <v>66</v>
+        <v>87</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -1174,74 +1217,96 @@
         <v>21</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C31" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="E31" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="H31" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="B32" s="6"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
+      <c r="A32" s="1">
         <v>22</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E33" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32" t="s">
+        <v>43</v>
+      </c>
+      <c r="E32" t="s">
+        <v>45</v>
+      </c>
+      <c r="H32" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33" s="9"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>23</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
+      </c>
+      <c r="C34" t="s">
+        <v>89</v>
       </c>
       <c r="E34" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="H34" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>24</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="E35" t="s">
-        <v>63</v>
+        <v>45</v>
+      </c>
+      <c r="H35" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>25</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C36" t="s">
+        <v>90</v>
+      </c>
+      <c r="E36" t="s">
+        <v>45</v>
+      </c>
+      <c r="H36" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="C2:H2"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:H6"/>
-    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C10:D10"/>
@@ -1251,6 +1316,16 @@
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="C4:D4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>